<commit_message>
Version mysql fonctionnelle, plus de CSV, reste a faire pareil pr JSON
</commit_message>
<xml_diff>
--- a/src/premium/Config/filtres_11.xlsx
+++ b/src/premium/Config/filtres_11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/remyadda/Desktop/AD/Projets/AD_serveur/src/premium/Config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC67AE2-7985-3F47-9CCD-A75904B233E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E980340D-BBD4-CA4D-BD95-3A3F82E47EC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" xr2:uid="{81B5A901-C830-ED4D-8852-1B248C2D9BB1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Nom - Prénom - Nom société</t>
   </si>
@@ -72,25 +72,19 @@
     <t>TYPE D'ENTREPRISE</t>
   </si>
   <si>
-    <t>Relations de 2e niveau;Relations de 3e niveau et plus</t>
-  </si>
-  <si>
     <t>France</t>
   </si>
   <si>
-    <t>Français</t>
-  </si>
-  <si>
     <t>Haddad - Eve - Etudiante</t>
   </si>
   <si>
     <t>Réseaux informatiques</t>
   </si>
   <si>
-    <t>Ressources humaines</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Relations de 3e niveau et plus</t>
   </si>
 </sst>
 </file>
@@ -459,8 +453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0DE78B2-A200-5F43-9BE1-DBB9550EE0FE}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -529,32 +523,30 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="E2" s="1"/>
       <c r="F2" s="2"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="1"/>
       <c r="M2" s="2"/>
       <c r="N2" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O2" s="1"/>
     </row>

</xml_diff>